<commit_message>
Fully Implemented [Needs Cleanup]
Looks like everything is working. Now more testing! Need to check file
selection, improper inputs, too many/few columns, blank rows, etc. Also
maybe more comments...
</commit_message>
<xml_diff>
--- a/ExceleratedSQL.xlsx
+++ b/ExceleratedSQL.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Aaron</t>
   </si>
@@ -58,39 +58,6 @@
   </si>
   <si>
     <t>Gruul</t>
-  </si>
-  <si>
-    <t>14/4/2001</t>
-  </si>
-  <si>
-    <t>14/4/2002</t>
-  </si>
-  <si>
-    <t>14/4/2003</t>
-  </si>
-  <si>
-    <t>14/4/2004</t>
-  </si>
-  <si>
-    <t>14/4/2005</t>
-  </si>
-  <si>
-    <t>14/4/2006</t>
-  </si>
-  <si>
-    <t>14/4/2007</t>
-  </si>
-  <si>
-    <t>14/4/2008</t>
-  </si>
-  <si>
-    <t>14/4/2009</t>
-  </si>
-  <si>
-    <t>14/4/2010</t>
-  </si>
-  <si>
-    <t>14/4/2011</t>
   </si>
   <si>
     <t>Kyle</t>
@@ -121,6 +88,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -150,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +420,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,8 +437,8 @@
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
+      <c r="B1" s="1">
+        <v>36995</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -486,8 +457,8 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
+      <c r="B2" s="1">
+        <v>36996</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -506,8 +477,8 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
+      <c r="B3" s="1">
+        <v>36997</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -526,14 +497,14 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
+      <c r="B4" s="1">
+        <v>36998</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>955281865</v>
@@ -546,14 +517,14 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
+      <c r="B5" s="1">
+        <v>36999</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>955281868</v>
@@ -566,14 +537,14 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
+      <c r="B6" s="1">
+        <v>37000</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <v>955281871</v>
@@ -586,14 +557,14 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
+      <c r="B7" s="1">
+        <v>37001</v>
       </c>
       <c r="C7">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E7">
         <v>955281874</v>
@@ -606,14 +577,14 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
+      <c r="B8" s="1">
+        <v>37002</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>955281877</v>
@@ -626,14 +597,14 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>22</v>
+      <c r="B9" s="1">
+        <v>37003</v>
       </c>
       <c r="C9">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>955281880</v>
@@ -646,14 +617,14 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
+      <c r="B10" s="1">
+        <v>37004</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <v>955281883</v>
@@ -666,14 +637,14 @@
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
+      <c r="B11" s="1">
+        <v>37005</v>
       </c>
       <c r="C11">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E11">
         <v>955281886</v>
@@ -684,6 +655,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>